<commit_message>
Added links to spreadsheet
</commit_message>
<xml_diff>
--- a/PRODUCTION/BOM.xlsx
+++ b/PRODUCTION/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\top_sneaky_part_2\Projects\devboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\top_sneaky_part_2\Projects\devboard\github\PRODUCTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D688EE16-7FC4-4500-912C-816589AE3AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875F0C12-6400-48E9-80B3-3871FA5A3C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12036" yWindow="2119" windowWidth="10406" windowHeight="10705" xr2:uid="{AC205121-B245-4684-9A00-34FE858BAD96}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{AC205121-B245-4684-9A00-34FE858BAD96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>Designator</t>
   </si>
@@ -270,16 +270,75 @@
   </si>
   <si>
     <t>Bill of Materials - Spreadsheet ver. (Everything from JLCPCB)</t>
+  </si>
+  <si>
+    <t>Link to JLCPCB page</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/26274-0402WGJ0103TCE/C25531</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/2358-RCMT08W270JT/C2006</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/26684-0402WGJ0512TCE/C25941</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/1877-CL05B104KO5NNNC/C1525</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/15107-CL05A105KP5NNNC/C14445</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/1914-0402CG330J500NT/C1562</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/2043-CL10A106MQ8NNNC/C1691</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/YXC_CrystalOscillators-X322512MSB4SI/C9002</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Korean_HropartsElec-TYPE_C_31_M12/C165948</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/244951-2_54_1_20P/C247921</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/HanElectricity-2541WR03P/C5383096</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/XUNPU-TS_1088AR02016/C720477</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/RaspberryPi-RP2040/C2040</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/JLCPCBAssembly-MCP1700/C9900006637</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/WinbondElec-W25Q16JVZPIQ/C377853</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,17 +361,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,29 +706,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1205EBA-E41F-4A90-AE0A-AC1FE2B81636}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.375" customWidth="1"/>
     <col min="3" max="3" width="45.625" customWidth="1"/>
     <col min="6" max="6" width="12.125" customWidth="1"/>
     <col min="7" max="7" width="17.875" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="22.625" customWidth="1"/>
+    <col min="11" max="11" width="68.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -675,11 +737,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -697,12 +759,15 @@
       <c r="J3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -717,12 +782,15 @@
       <c r="J4">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
@@ -737,8 +805,11 @@
       <c r="J5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -757,12 +828,15 @@
       <c r="J6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
@@ -777,12 +851,15 @@
       <c r="J7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
@@ -797,12 +874,15 @@
       <c r="J8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" t="s">
@@ -817,12 +897,15 @@
       <c r="J9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="s">
@@ -837,12 +920,15 @@
       <c r="J10">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="C11" t="s">
@@ -857,12 +943,15 @@
       <c r="J11">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
@@ -877,12 +966,15 @@
       <c r="J12">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>41</v>
       </c>
       <c r="C13" t="s">
@@ -897,12 +989,15 @@
       <c r="J13">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" t="s">
@@ -917,12 +1012,15 @@
       <c r="J14">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
@@ -937,12 +1035,15 @@
       <c r="J15">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>56</v>
       </c>
       <c r="C16" t="s">
@@ -957,12 +1058,15 @@
       <c r="J16">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>61</v>
       </c>
       <c r="C17" t="s">
@@ -977,12 +1081,15 @@
       <c r="J17">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>65</v>
       </c>
       <c r="C18" t="s">
@@ -997,12 +1104,15 @@
       <c r="J18">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>70</v>
       </c>
       <c r="C19" t="s">
@@ -1017,8 +1127,29 @@
       <c r="J19">
         <v>0.35</v>
       </c>
+      <c r="K19" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{65A31AF7-6895-4443-A3CA-6C4B7FAFA5D2}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{1923E332-B697-41EB-9A34-9FDA5B496FCD}"/>
+    <hyperlink ref="K6" r:id="rId3" xr:uid="{E3100AE8-1D4C-4792-98A7-99A5CCA1F45E}"/>
+    <hyperlink ref="K7" r:id="rId4" xr:uid="{4BC1FCA7-9830-4566-A2A5-E1ADE72EA105}"/>
+    <hyperlink ref="K8" r:id="rId5" xr:uid="{1F12A23B-83C4-4202-8C8B-66B5B35BFD50}"/>
+    <hyperlink ref="K9" r:id="rId6" xr:uid="{53B54977-5450-4DE9-A623-E94B9A243574}"/>
+    <hyperlink ref="K10" r:id="rId7" xr:uid="{036F1E72-E1AD-4C10-BD1F-5DF4B5777CE9}"/>
+    <hyperlink ref="K11" r:id="rId8" xr:uid="{92428A5E-3220-43E8-BC96-4E3A9DCB05C8}"/>
+    <hyperlink ref="K12" r:id="rId9" xr:uid="{640D486B-3EEC-4082-AB16-4D0A09FE262E}"/>
+    <hyperlink ref="K13" r:id="rId10" xr:uid="{769B2375-E843-491B-AF04-2B55206A1EF1}"/>
+    <hyperlink ref="K14" r:id="rId11" xr:uid="{A8A48E89-CF74-43ED-B027-106B347A159C}"/>
+    <hyperlink ref="K15" r:id="rId12" xr:uid="{E34A3978-05AB-49BB-AE37-8F1ACE2C7791}"/>
+    <hyperlink ref="K16" r:id="rId13" xr:uid="{543A3896-65FD-45CA-95D8-83126A8E5468}"/>
+    <hyperlink ref="K17" r:id="rId14" xr:uid="{8CFFCFF7-848D-428A-B6B3-D25A148D101C}"/>
+    <hyperlink ref="K18" r:id="rId15" xr:uid="{4DDDC750-423D-414B-BF8F-85FCE0796D8D}"/>
+    <hyperlink ref="K19" r:id="rId16" xr:uid="{1DAFE810-6764-4D6A-AB63-A839F02DAA32}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>